<commit_message>
Stock hasta el punto pedido por la empresa
Hasta acá me pidió la empresa.
</commit_message>
<xml_diff>
--- a/Functionalities/Stock/data/dummy_stock.xlsx
+++ b/Functionalities/Stock/data/dummy_stock.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>item</t>
   </si>
@@ -23,94 +23,85 @@
     <t>stock</t>
   </si>
   <si>
-    <t>item_0</t>
-  </si>
-  <si>
-    <t>item_1</t>
-  </si>
-  <si>
-    <t>item_2</t>
-  </si>
-  <si>
-    <t>item_3</t>
-  </si>
-  <si>
-    <t>item_4</t>
-  </si>
-  <si>
-    <t>item_5</t>
-  </si>
-  <si>
-    <t>item_6</t>
-  </si>
-  <si>
-    <t>item_7</t>
-  </si>
-  <si>
-    <t>item_8</t>
-  </si>
-  <si>
-    <t>item_9</t>
-  </si>
-  <si>
-    <t>item_10</t>
-  </si>
-  <si>
-    <t>item_11</t>
-  </si>
-  <si>
-    <t>item_12</t>
-  </si>
-  <si>
-    <t>item_13</t>
-  </si>
-  <si>
-    <t>item_14</t>
-  </si>
-  <si>
-    <t>item_15</t>
-  </si>
-  <si>
-    <t>item_16</t>
-  </si>
-  <si>
-    <t>item_17</t>
-  </si>
-  <si>
-    <t>item_18</t>
-  </si>
-  <si>
-    <t>item_19</t>
-  </si>
-  <si>
-    <t>item_20</t>
-  </si>
-  <si>
-    <t>item_21</t>
-  </si>
-  <si>
-    <t>item_22</t>
-  </si>
-  <si>
-    <t>item_23</t>
-  </si>
-  <si>
-    <t>item_24</t>
-  </si>
-  <si>
-    <t>item_25</t>
-  </si>
-  <si>
-    <t>item_26</t>
-  </si>
-  <si>
-    <t>item_27</t>
-  </si>
-  <si>
-    <t>item_28</t>
-  </si>
-  <si>
-    <t>item_29</t>
+    <t>MCER017</t>
+  </si>
+  <si>
+    <t>MCER018</t>
+  </si>
+  <si>
+    <t>MCER020</t>
+  </si>
+  <si>
+    <t>MCER021</t>
+  </si>
+  <si>
+    <t>MCER022</t>
+  </si>
+  <si>
+    <t>MCER026</t>
+  </si>
+  <si>
+    <t>MCER027</t>
+  </si>
+  <si>
+    <t>MCER028</t>
+  </si>
+  <si>
+    <t>MCER029</t>
+  </si>
+  <si>
+    <t>MCER030</t>
+  </si>
+  <si>
+    <t>MCER031</t>
+  </si>
+  <si>
+    <t>MCER032</t>
+  </si>
+  <si>
+    <t>MCER033</t>
+  </si>
+  <si>
+    <t>MCER034</t>
+  </si>
+  <si>
+    <t>MCER035</t>
+  </si>
+  <si>
+    <t>MCER036</t>
+  </si>
+  <si>
+    <t>MCER037</t>
+  </si>
+  <si>
+    <t>MCER038</t>
+  </si>
+  <si>
+    <t>MCER039</t>
+  </si>
+  <si>
+    <t>MCER040</t>
+  </si>
+  <si>
+    <t>MCER041</t>
+  </si>
+  <si>
+    <t>MCER043</t>
+  </si>
+  <si>
+    <t>MCER046</t>
+  </si>
+  <si>
+    <t>MCER047</t>
+  </si>
+  <si>
+    <t>MCER051</t>
+  </si>
+  <si>
+    <t>MCER057</t>
+  </si>
+  <si>
+    <t>MCER067</t>
   </si>
 </sst>
 </file>
@@ -468,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -698,30 +689,6 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>821</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -729,7 +696,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -748,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>177</v>
+        <v>890</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -756,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>988</v>
+        <v>837</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -764,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>499</v>
+        <v>821</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -772,7 +739,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>758</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -780,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>939</v>
+        <v>988</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -788,7 +755,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>602</v>
+        <v>499</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -796,7 +763,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>250</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -804,7 +771,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>170</v>
+        <v>939</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -812,7 +779,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>188</v>
+        <v>602</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -820,7 +787,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>890</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -828,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -836,7 +803,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>542</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -844,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>223</v>
+        <v>890</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -852,7 +819,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>889</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -860,7 +827,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>800</v>
+        <v>542</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -868,7 +835,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>146</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -876,7 +843,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>805</v>
+        <v>889</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -884,7 +851,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>973</v>
+        <v>800</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -892,7 +859,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>648</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -900,7 +867,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>850</v>
+        <v>805</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -908,7 +875,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>818</v>
+        <v>973</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -916,7 +883,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>710</v>
+        <v>648</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -924,7 +891,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>439</v>
+        <v>850</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -932,7 +899,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>16</v>
+        <v>818</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -940,7 +907,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>731</v>
+        <v>710</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -948,7 +915,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>207</v>
+        <v>439</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -956,31 +923,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31">
-        <v>254</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>